<commit_message>
main - Update no problems with duplicate codes
</commit_message>
<xml_diff>
--- a/agregar_productos.xlsx
+++ b/agregar_productos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>code</t>
   </si>
@@ -110,7 +110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -121,6 +121,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,12 +141,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,6 +512,33 @@
         <v>30</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>3.8000924422E10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>3.8000924422E10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>3.8000924422E10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>